<commit_message>
feat. narration skip & quiz check
</commit_message>
<xml_diff>
--- a/WhiteCane/Assets/Resources/Xlsx/NarrationData.xlsx
+++ b/WhiteCane/Assets/Resources/Xlsx/NarrationData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WhiteCane\WhiteCane\Assets\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WhiteCane\WhiteCane\Assets\Resources\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,32 +42,139 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Test_Narration_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test_Narration_02</t>
-  </si>
-  <si>
-    <t>Test_Narration_03</t>
-  </si>
-  <si>
-    <t>Test_Narration_04</t>
-  </si>
-  <si>
-    <t>씬 시작 멘트 입니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>narration data에 있습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3번 나레이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4번 나레이션</t>
+    <t>intro_02</t>
+  </si>
+  <si>
+    <t>foreset_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여러분은 현재 드넓은 숲 한가운데에 서 있습니다.</t>
+  </si>
+  <si>
+    <t>이곳에서 나가기 위해서는 폭포를 찾아가야합니다.</t>
+  </si>
+  <si>
+    <t>소리를 듣고 소리의 정체가 무엇인지 맞추면 되는 간단한 퀴즈입니다.</t>
+  </si>
+  <si>
+    <t>답을 맞추시면 폭포 위치에 대한 힌트를 얻을 수 있습니다.</t>
+  </si>
+  <si>
+    <t>foreset_02</t>
+  </si>
+  <si>
+    <t>foreset_03</t>
+  </si>
+  <si>
+    <t>foreset_04</t>
+  </si>
+  <si>
+    <t>foreset_05</t>
+  </si>
+  <si>
+    <t>foreset_06</t>
+  </si>
+  <si>
+    <t>폭포를 찾아가는 길에는 예상치 못한 퀴즈들이 기다리고 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한번해볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial02</t>
+  </si>
+  <si>
+    <t>tutorial03</t>
+  </si>
+  <si>
+    <t>tutorial06</t>
+  </si>
+  <si>
+    <t>tutorial07</t>
+  </si>
+  <si>
+    <t>tutorial08</t>
+  </si>
+  <si>
+    <t>foreset_07</t>
+  </si>
+  <si>
+    <t>이제 폭포소리를 따라 발걸음을 옮겨주시기를 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>즐거운 여정이 되시길 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>whitecane에 오신 여러분 환영합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금부터 여러분의 시각 일부를 제한하고 청각과 촉감에 의존하여 떠나는 색다른 모험으로 안내하겠습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작하기 앞서 게임의 방법을 소개해드리겠습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물체를 맞추는 방법에 대해 알려드리겠습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a를 꾹 눌러 녹음을 진행하고 버튼을 땝니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘하셨습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이제 지팡이를 드리겠습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지팡이가 닿는 곳은 부분적으로 밝아집니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앞에 무엇이 잇는지 몰라 망설여질 때 유용하게 활용해보세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소리가 들리는 곳으로 발걸음을 옮겨주시기를 바랍니다. 즐거운 여정이 되시길 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intro_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>즐거운 여정이 되시길 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -409,7 +516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -418,7 +525,7 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.25" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="3" max="3" width="92.625" customWidth="1"/>
     <col min="4" max="4" width="17.25" customWidth="1"/>
     <col min="5" max="5" width="12.75" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
@@ -445,35 +552,155 @@
     </row>
     <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat. final quiz scene
</commit_message>
<xml_diff>
--- a/WhiteCane/Assets/Resources/Xlsx/NarrationData.xlsx
+++ b/WhiteCane/Assets/Resources/Xlsx/NarrationData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
   <si>
     <t>array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,156 +78,340 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>개는 사람들에게 사랑과 충성심을 보여줍니다. 이처럼 사람들과의 관계에서 더 많은 사랑과 신뢰를 쌓는 데 중요합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial09</t>
+  </si>
+  <si>
+    <t>tutorial10</t>
+  </si>
+  <si>
+    <t>tutorial11</t>
+  </si>
+  <si>
+    <t>tutorial12</t>
+  </si>
+  <si>
+    <t>tutorial13</t>
+  </si>
+  <si>
+    <t>tutorial14</t>
+  </si>
+  <si>
+    <t>tutorial15</t>
+  </si>
+  <si>
+    <t>감각의 공간 리소니아에 오신 것을 환영합니다. 이곳은 시각을 제외한 감각들로 느끼는 세상입니다. 보이지 않는 것을 다른 감각으로 채워나갈 때 비로소 여러분만의 리소니아가 완성됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저는 이곳의 안내자 오스카입니다. 어둠 속에서 길을 잃지 않도록 제가 잘 안내해 드리겠습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 방식을 설명해 드리겠습니다. 제 안내를 따라 오른쪽 컨트롤러의 조이스틱을 이용하여 이동하시면 됩니다. 길을 잘못 들었을 때는 저를 호출하실 수 있는 버튼이 생성됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>길을 잘못 들었을 때는 저를 호출하실 수 있는 버튼이 생성됩니다. 오른쪽 콘트롤러의 b 버튼을 누르시면 제가 다시 올바른 길로 안내해 드리겠습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리소니아는 5개의 구역으로 이루어져 있고, 각 구역에는 여러분을 기다리고 있는 생명체들이 있습니다. 리소니아를 여행하며 이들과 관련된 퀴즈를 풀어보세요. 5개의 생명력은 감각의 세상을 완성하고 균형과 조화 속에서 이 세상을 지탱할 것입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자, 오른쪽 컨트롤러의 그립버튼으로 눈앞에 보이는 지팡이를 잡아볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a 버튼을 눌러 말하고 a버튼을 때면 음성 인식이 완료됩니다. 한번 해볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>이 동물은 무엇일까요?</t>
-  </si>
-  <si>
-    <t>개는 사람들에게 사랑과 충성심을 보여줍니다. 이처럼 사람들과의 관계에서 더 많은 사랑과 신뢰를 쌓는 데 중요합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘하셨습니다. 만나본 동물은 개 입니다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>잘하셨습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주변이 보이지 않아 발걸음을 떼기가 망설여진다면 지팡이를 땅에 두드리시면 됩니다. 주변이 잠시 밝아질 겁니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘하셨습니다. 이제 리소니아로 떠나 볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tutorial01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forest03</t>
+  </si>
+  <si>
+    <t>forest04</t>
+  </si>
+  <si>
+    <t>forest05</t>
+  </si>
+  <si>
+    <t>forest06</t>
+  </si>
+  <si>
+    <t>forest07</t>
+  </si>
+  <si>
+    <t>deepSea01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deepSea02</t>
+  </si>
+  <si>
+    <t>deepSea04</t>
+  </si>
+  <si>
+    <t>deepSea06</t>
+  </si>
+  <si>
+    <t>deepSea07</t>
+  </si>
+  <si>
+    <t>deepSea08</t>
+  </si>
+  <si>
+    <t>deepSea09</t>
+  </si>
+  <si>
+    <t>deepSea10</t>
+  </si>
+  <si>
+    <t>cooperation02</t>
+  </si>
+  <si>
+    <t>cooperation03</t>
+  </si>
+  <si>
+    <t>cooperation04</t>
+  </si>
+  <si>
+    <t>cooperation05</t>
+  </si>
+  <si>
+    <t>cooperation06</t>
+  </si>
+  <si>
+    <t>cooperation07</t>
+  </si>
+  <si>
+    <t>cooperation08</t>
+  </si>
+  <si>
+    <t>memories02</t>
+  </si>
+  <si>
+    <t>memories03</t>
+  </si>
+  <si>
+    <t>memories04</t>
+  </si>
+  <si>
+    <t>memories05</t>
+  </si>
+  <si>
+    <t>bamboo02</t>
+  </si>
+  <si>
+    <t>bamboo04</t>
+  </si>
+  <si>
+    <t>bamboo05</t>
+  </si>
+  <si>
+    <t>bamboo06</t>
+  </si>
+  <si>
+    <t>bamboo07</t>
   </si>
   <si>
     <t>이곳은 소통의 숲입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이 곳에서는 사람들에게 도움을 주는 동물을 만나볼 수 있습니다</t>
-  </si>
-  <si>
-    <t>tutorial09</t>
-  </si>
-  <si>
-    <t>tutorial10</t>
-  </si>
-  <si>
-    <t>tutorial11</t>
-  </si>
-  <si>
-    <t>tutorial12</t>
-  </si>
-  <si>
-    <t>tutorial13</t>
-  </si>
-  <si>
-    <t>tutorial14</t>
-  </si>
-  <si>
-    <t>tutorial15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 동물은 무엇일까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>잘하셨습니다. 만나본 동물은 소 입니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>소는 사람들과 함께 농장에서 일하며 인내력이 강합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이처럼 인내와 끈기를 통해 꾸준히 노력하면 목표를 이룰 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이제 다음 장소로 이동해볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>바닷가에 오신걸 환영합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳에 사는 존재들을 더 가까이서 만나기 위해 바닷속으로 들어가볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳은 지혜의 심해입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳에서는 소리로 소통하는 거대한 크기의 동물을 만나볼 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 동물은 무엇일까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘하셨습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>만나본 동물은 고래입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>고래는 경험과 지식을 공유하여 지혜롭게 살아갑니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이러한 지혜를 통해 새로운 상황에 적절하게 대응할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이제 다시 숲으로 돌아가보겠습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳은 대나무의 숲 입니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳에서는 특이한 외모와 순한 성격으로 사람들에게 사랑받는 동물을 만나볼 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘하셨습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>만나본 동물은 팬더입니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>팬더는 위협을 느끼지 않는다면 주로 온화하게 행동합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이처럼 불필요한 갈등을 피하고, 평화와 조화를 추구하는 것이 중요합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이제 더 깊은 숲속으로 걸어가겠습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳은 협력의 숲입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳에서는 사회적인 관계를 통해 살아가는 동물을 만날 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 동물은 무엇일까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>만나본 동물은 늑대입니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>늑대들은 무리를 지어 함께 살아갑니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이제 숲을 벗어나 마지막 장소인 초원으로 이동해볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이처럼 혼자서 할 수 없는 일도 협력하면 이룰 수 있습니다.</t>
-  </si>
-  <si>
-    <t>이제 숲을 벗어나 마지막 장소인 초원으로 이동해볼까요?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>여기까지 오시느라 고생많으셨습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳은 기억의 초원으로 마지막 장소입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이곳에서는 뛰어난 기억력으로 사람들에게 놀라움을 주는 동물을 만나볼 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 동물은 무엇일까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>잘하셨습니다. 마지막으로 만나신 존재는 앵무새입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>의미있는 시간을 보내셨나요? 기억력이 좋은 앵무새가 이곳에서 여러분과 함께했던 행복한 기억들을 오랫동안 간직해줄 것입니다.</t>
-  </si>
-  <si>
-    <t>감각의 공간 리소니아에 오신 것을 환영합니다. 이곳은 시각을 제외한 감각들로 느끼는 세상입니다. 보이지 않는 것을 다른 감각으로 채워나갈 때 비로소 여러분만의 리소니아가 완성됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>저는 이곳의 안내자 오스카입니다. 어둠 속에서 길을 잃지 않도록 제가 잘 안내해 드리겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 방식을 설명해 드리겠습니다. 제 안내를 따라 오른쪽 컨트롤러의 조이스틱을 이용하여 이동하시면 됩니다. 길을 잘못 들었을 때는 저를 호출하실 수 있는 버튼이 생성됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>길을 잘못 들었을 때는 저를 호출하실 수 있는 버튼이 생성됩니다. 오른쪽 콘트롤러의 b 버튼을 누르시면 제가 다시 올바른 길로 안내해 드리겠습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리소니아는 5개의 구역으로 이루어져 있고, 각 구역에는 여러분을 기다리고 있는 생명체들이 있습니다. 리소니아를 여행하며 이들과 관련된 퀴즈를 풀어보세요. 5개의 생명력은 감각의 세상을 완성하고 균형과 조화 속에서 이 세상을 지탱할 것입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자, 오른쪽 컨트롤러의 그립버튼으로 눈앞에 보이는 지팡이를 잡아볼까요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a 버튼을 눌러 말하고 a버튼을 때면 음성 인식이 완료됩니다. 한번 해볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memories06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forest01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forest02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deepSea03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deepSea05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bamboo01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -235,143 +419,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>잘하셨습니다. 만나본 동물은 개 입니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘하셨습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주변이 보이지 않아 발걸음을 떼기가 망설여진다면 지팡이를 땅에 두드리시면 됩니다. 주변이 잠시 밝아질 겁니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘하셨습니다. 이제 리소니아로 떠나 볼까요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tutorial01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>forest01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>forest02</t>
-  </si>
-  <si>
-    <t>forest03</t>
-  </si>
-  <si>
-    <t>forest04</t>
-  </si>
-  <si>
-    <t>forest05</t>
-  </si>
-  <si>
-    <t>forest06</t>
-  </si>
-  <si>
-    <t>forest07</t>
-  </si>
-  <si>
-    <t>deepSea01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>deepSea02</t>
-  </si>
-  <si>
-    <t>deepSea03</t>
-  </si>
-  <si>
-    <t>deepSea04</t>
-  </si>
-  <si>
-    <t>deepSea05</t>
-  </si>
-  <si>
-    <t>deepSea06</t>
-  </si>
-  <si>
-    <t>deepSea07</t>
-  </si>
-  <si>
-    <t>deepSea08</t>
-  </si>
-  <si>
-    <t>deepSea09</t>
-  </si>
-  <si>
-    <t>deepSea10</t>
+    <t>bamboo03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bamboo08</t>
+  </si>
+  <si>
+    <t>cooperation01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>memories01</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cooperation01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cooperation02</t>
-  </si>
-  <si>
-    <t>cooperation03</t>
-  </si>
-  <si>
-    <t>cooperation04</t>
-  </si>
-  <si>
-    <t>cooperation05</t>
-  </si>
-  <si>
-    <t>cooperation06</t>
-  </si>
-  <si>
-    <t>cooperation07</t>
-  </si>
-  <si>
-    <t>cooperation08</t>
-  </si>
-  <si>
-    <t>memories02</t>
-  </si>
-  <si>
-    <t>memories03</t>
-  </si>
-  <si>
-    <t>memories04</t>
-  </si>
-  <si>
-    <t>memories05</t>
-  </si>
-  <si>
-    <t>memories06</t>
-  </si>
-  <si>
-    <t>bamboo01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bamboo02</t>
-  </si>
-  <si>
-    <t>bamboo03</t>
-  </si>
-  <si>
-    <t>bamboo04</t>
-  </si>
-  <si>
-    <t>bamboo05</t>
-  </si>
-  <si>
-    <t>bamboo06</t>
-  </si>
-  <si>
-    <t>bamboo07</t>
   </si>
 </sst>
 </file>
@@ -423,11 +483,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -746,10 +809,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -757,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -765,7 +828,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -773,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -781,7 +844,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -789,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -805,12 +868,12 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -818,354 +881,362 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>15</v>
+      <c r="B37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" t="s">
-        <v>39</v>
+      <c r="B38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>102</v>
-      </c>
-      <c r="C39" t="s">
-        <v>40</v>
+      <c r="B39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" t="s">
-        <v>41</v>
+      <c r="B40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" t="s">
-        <v>42</v>
+      <c r="B41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" t="s">
-        <v>43</v>
+      <c r="B42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
         <v>90</v>
-      </c>
-      <c r="C47" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
         <v>91</v>
-      </c>
-      <c r="C48" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>